<commit_message>
Some small gui tweaks.  The biggest change was to roll back the built-in stlink firmware which made everything work again.
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="67">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco DCC LCC</t>
   </si>
 </sst>
 </file>
@@ -1431,6 +1440,9 @@
       <c r="I3" s="21" t="s">
         <v>36</v>
       </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -1451,6 +1463,7 @@
         <v>48</v>
       </c>
       <c r="I4"/>
+      <c r="J4"/>
       <c r="K4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1680,7 +1693,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="2:10"/>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="7" spans="2:10"/>
     <row r="8" spans="2:10"/>
     <row r="9" spans="2:10"/>

</xml_diff>

<commit_message>
Support external bitmaps.  Png files only (24bit,no transparency) are converted to .bin (width16,height16,format8,data) on first use.
Restore SDIO TX DMA (rx and tx dma stream shared)
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="69">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t xml:space="preserve">Disco DCC LCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1701,7 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Add some ui buttons.  Link to preferences.
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="96">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -224,6 +224,87 @@
   </si>
   <si>
     <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function Key1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function Key5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function Key4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function Key3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function Key2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the status bar - power, clock, connection status, events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,a-z,A-Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`~!@#$%^&amp;*()_+-={}|[]\&lt;&gt;?,./</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`~!@#$%^&amp;*()_+-={}|[]\&lt;&gt;?,./"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`~!@#$%^&amp;*()_+-={}|[]\&lt;&gt;?,./"';:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardTextId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`~!@ #$%^&amp;*()_+-={}|[]\&lt;&gt;?,./"';:</t>
   </si>
 </sst>
 </file>
@@ -1487,7 +1568,29 @@
       </c>
     </row>
     <row r="5" spans="2:15">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
       <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1667,16 +1770,16 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
         <v>59</v>
@@ -1684,16 +1787,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -1701,25 +1804,123 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="2:10"/>
-    <row r="8" spans="2:10"/>
-    <row r="9" spans="2:10"/>
-    <row r="10" spans="2:10"/>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="13" spans="2:10"/>
     <row r="14" spans="2:10"/>
     <row r="15" spans="2:10"/>

</xml_diff>

<commit_message>
Add model/view initial implementation for dccsettings
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2369" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3246" uniqueCount="124">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -305,6 +305,90 @@
   </si>
   <si>
     <t xml:space="preserve">`~!@ #$%^&amp;*()_+-={}|[]\&lt;&gt;?,./"';:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trip Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***&lt;value&gt;***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx&lt;value&gt;xxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardTextIdCenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slew Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prog.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backlight</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1880,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>59</v>
@@ -1804,16 +1888,16 @@
     </row>
     <row r="6" spans="2:10">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
         <v>59</v>
@@ -1821,7 +1905,7 @@
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
         <v>69</v>
@@ -1838,16 +1922,16 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
@@ -1855,16 +1939,16 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
         <v>59</v>
@@ -1872,16 +1956,16 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
         <v>59</v>
@@ -1889,16 +1973,16 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
         <v>59</v>
@@ -1906,7 +1990,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>69</v>
@@ -1915,18 +1999,114 @@
         <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="F12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="2:10"/>
-    <row r="14" spans="2:10"/>
-    <row r="15" spans="2:10"/>
-    <row r="16" spans="2:10"/>
-    <row r="17" spans="4:4"/>
-    <row r="18" spans="4:4"/>
+    <row r="13" spans="2:10">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="19" spans="4:4"/>
     <row r="20" spans="4:4"/>
     <row r="21" spans="4:4"/>

</xml_diff>

<commit_message>
Add full keyboard and numeric keypad
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6766" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10283" uniqueCount="190">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -482,6 +482,111 @@
   </si>
   <si>
     <t xml:space="preserve">wildcardTextIdMedium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_Numeric_40px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consola.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardTextIdMediumNumeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decoder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigDecoder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigConfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All CVs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DccConfigAllCVs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardTextIdNumeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;id&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!”"#*%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!”#*"%&amp;()'$+-@_, .:;?/~±×÷•º`´{}©£€^®¥_=[]¡¢|\¿&gt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnteredText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;placeHolder&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlphaMode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123</t>
   </si>
 </sst>
 </file>
@@ -1832,7 +1937,9 @@
       <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="G7"/>
+      <c r="G7" t="s">
+        <v>182</v>
+      </c>
       <c r="H7" t="s">
         <v>137</v>
       </c>
@@ -1855,6 +1962,27 @@
       </c>
     </row>
     <row r="8" spans="2:15">
+      <c r="B8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="8" t="s">
         <v>16</v>
       </c>
@@ -1870,6 +1998,29 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="2:15">
+      <c r="B9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>180</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
       <c r="K9" s="12" t="s">
         <v>14</v>
       </c>
@@ -1887,6 +2038,29 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="12" t="s">
         <v>36</v>
       </c>
@@ -1902,6 +2076,25 @@
       <c r="O10" s="15"/>
     </row>
     <row r="11" spans="2:15">
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" s="16"/>
     </row>
     <row r="12" spans="2:15">
@@ -2392,17 +2585,193 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="4:4"/>
-    <row r="29" spans="4:4"/>
-    <row r="30" spans="4:4"/>
-    <row r="31" spans="4:4"/>
-    <row r="32" spans="4:4"/>
-    <row r="33" spans="4:4"/>
-    <row r="34" spans="4:4"/>
-    <row r="35" spans="4:4"/>
-    <row r="36" spans="4:4"/>
-    <row r="37" spans="4:4"/>
-    <row r="38" spans="4:4"/>
+    <row r="28" spans="4:4">
+      <c r="B28" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="B29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="B30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="B32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>166</v>
+      </c>
+      <c r="F32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="B33" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>168</v>
+      </c>
+      <c r="F33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="B34" t="s">
+        <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="B35" t="s">
+        <v>176</v>
+      </c>
+      <c r="C35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4">
+      <c r="B36" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4">
+      <c r="B37" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="B38" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="39" spans="4:4"/>
     <row r="40" spans="4:4"/>
     <row r="41" spans="4:4"/>

</xml_diff>

<commit_message>
Add audio settings - just mute for now
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17616" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17866" uniqueCount="210">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2526,16 +2526,16 @@
     </row>
     <row r="24" spans="4:4">
       <c r="B24" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="C24" t="s">
         <v>201</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="F24" t="s">
         <v>59</v>
@@ -2543,16 +2543,16 @@
     </row>
     <row r="25" spans="4:4">
       <c r="B25" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="C25" t="s">
         <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
@@ -2560,16 +2560,16 @@
     </row>
     <row r="26" spans="4:4">
       <c r="B26" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C26" t="s">
         <v>201</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F26" t="s">
         <v>59</v>
@@ -2577,7 +2577,7 @@
     </row>
     <row r="27" spans="4:4">
       <c r="B27" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
         <v>201</v>
@@ -2586,7 +2586,7 @@
         <v>62</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F27" t="s">
         <v>59</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="28" spans="4:4">
       <c r="B28" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
         <v>201</v>
@@ -2603,7 +2603,7 @@
         <v>62</v>
       </c>
       <c r="E28" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
         <v>59</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="29" spans="4:4">
       <c r="B29" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C29" t="s">
         <v>201</v>
@@ -2620,7 +2620,7 @@
         <v>62</v>
       </c>
       <c r="E29" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="F29" t="s">
         <v>59</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="30" spans="4:4">
       <c r="B30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C30" t="s">
         <v>201</v>
@@ -2637,7 +2637,7 @@
         <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F30" t="s">
         <v>59</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="31" spans="4:4">
       <c r="B31" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C31" t="s">
         <v>201</v>
@@ -2654,7 +2654,7 @@
         <v>62</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="F31" t="s">
         <v>59</v>
@@ -2662,16 +2662,16 @@
     </row>
     <row r="32" spans="4:4">
       <c r="B32" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D32" t="s">
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F32" t="s">
         <v>59</v>
@@ -2679,16 +2679,16 @@
     </row>
     <row r="33" spans="4:4">
       <c r="B33" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D33" t="s">
         <v>62</v>
       </c>
       <c r="E33" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F33" t="s">
         <v>59</v>
@@ -2696,16 +2696,16 @@
     </row>
     <row r="34" spans="4:4">
       <c r="B34" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D34" t="s">
         <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F34" t="s">
         <v>59</v>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="35" spans="4:4">
       <c r="B35" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C35" t="s">
         <v>198</v>
@@ -2722,7 +2722,7 @@
         <v>62</v>
       </c>
       <c r="E35" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F35" t="s">
         <v>59</v>
@@ -2730,16 +2730,16 @@
     </row>
     <row r="36" spans="4:4">
       <c r="B36" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D36" t="s">
         <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>46</v>
       </c>
       <c r="F36" t="s">
         <v>59</v>
@@ -2747,16 +2747,16 @@
     </row>
     <row r="37" spans="4:4">
       <c r="B37" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
       <c r="F37" t="s">
         <v>59</v>
@@ -2764,16 +2764,16 @@
     </row>
     <row r="38" spans="4:4">
       <c r="B38" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D38" t="s">
         <v>58</v>
       </c>
       <c r="E38" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F38" t="s">
         <v>59</v>
@@ -2781,16 +2781,16 @@
     </row>
     <row r="39" spans="4:4">
       <c r="B39" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
         <v>58</v>
       </c>
       <c r="E39" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F39" t="s">
         <v>59</v>
@@ -2798,16 +2798,16 @@
     </row>
     <row r="40" spans="4:4">
       <c r="B40" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
         <v>201</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s">
-        <v>209</v>
+        <v>148</v>
       </c>
       <c r="F40" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Add custom icons/images for decoders.
</commit_message>
<xml_diff>
--- a/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
+++ b/STM32F469_Controller/Source/TouchGFX/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19164" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19438" uniqueCount="220">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t xml:space="preserve">DCCConfigLargeImage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wildcardTextCentered28pxId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;placeholder&gt;</t>
   </si>
 </sst>
 </file>
@@ -2888,7 +2894,23 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="4:4"/>
+    <row r="44" spans="4:4">
+      <c r="B44" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>219</v>
+      </c>
+      <c r="F44" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="45" spans="4:4"/>
     <row r="46" spans="4:4"/>
     <row r="47" spans="4:4"/>

</xml_diff>